<commit_message>
update of archetype files
</commit_message>
<xml_diff>
--- a/data/aggregate.xlsx
+++ b/data/aggregate.xlsx
@@ -1,23 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n/code/BuildME/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrenis\gitprojects\BuildME\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEB78A6-89C6-4E49-8556-C631A2717EB5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF20039B-D27B-429E-8ABA-8C309B67F48E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-11920" windowWidth="21560" windowHeight="23540" xr2:uid="{464E4639-C8DD-E743-AA72-67524FC7DCD8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{464E4639-C8DD-E743-AA72-67524FC7DCD8}"/>
   </bookViews>
   <sheets>
     <sheet name="climate_reg" sheetId="2" r:id="rId1"/>
-    <sheet name="energy_carrier" sheetId="3" r:id="rId2"/>
-    <sheet name="USA_Peter_climatereg" sheetId="1" r:id="rId3"/>
+    <sheet name="New_regions_climate_reg" sheetId="4" r:id="rId2"/>
+    <sheet name="energy_carrier" sheetId="3" r:id="rId3"/>
+    <sheet name="USA_Peter_climatereg" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="17" r:id="rId5"/>
+    <pivotCache cacheId="11" r:id="rId6"/>
+    <pivotCache cacheId="8" r:id="rId7"/>
+    <pivotCache cacheId="5" r:id="rId8"/>
+    <pivotCache cacheId="20" r:id="rId9"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,6 +33,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="98">
   <si>
     <t>1A-2A</t>
   </si>
@@ -242,16 +251,101 @@
   </si>
   <si>
     <t>JP8</t>
+  </si>
+  <si>
+    <t>Moscow</t>
+  </si>
+  <si>
+    <t>Karachi/Islamabad/Kabul</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Busan/Seoul</t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Johannesburg</t>
+  </si>
+  <si>
+    <t>Tel Aviv</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Istanbul</t>
+  </si>
+  <si>
+    <t>Mexico city</t>
+  </si>
+  <si>
+    <t>Zurich</t>
+  </si>
+  <si>
+    <t>R5.2OECD_Other</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Sum of disagg building stock</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>R5.2REF_Other</t>
+  </si>
+  <si>
+    <t>Samarkand</t>
+  </si>
+  <si>
+    <t>R5.2ASIA_Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teheran </t>
+  </si>
+  <si>
+    <t>R5.2LAM_Other</t>
+  </si>
+  <si>
+    <t>See Modeling/RECC-buildings/Mapping_climate_RECC_regions.xlsx</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>Oth-OECD</t>
+  </si>
+  <si>
+    <t>Oth-REF</t>
+  </si>
+  <si>
+    <t>Oth-Asia</t>
+  </si>
+  <si>
+    <t>Oth-MAF</t>
+  </si>
+  <si>
+    <t>Oth-LAM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0\ %"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -280,6 +374,20 @@
       <name val="ArialMT"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="ArialMT"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -302,7 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -315,12 +423,29 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0\ %"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0\ %"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0\ %"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0\ %"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -331,6 +456,1065 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Andrea A. Nistad" refreshedDate="43965.628342939817" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="36" xr:uid="{DE82C6EC-F927-464E-A2EA-72716E065F4A}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="E145:F181" sheet="aggregation_stock" r:id="rId2"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="disagg building stock" numFmtId="9">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="0.42584040981210575"/>
+    </cacheField>
+    <cacheField name="climate reg" numFmtId="0">
+      <sharedItems count="1">
+        <s v="RIO"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Andrea A. Nistad" refreshedDate="43965.62732511574" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="31" xr:uid="{8864F91D-6E7B-4126-BF47-4634A95B9609}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="E41:F72" sheet="aggregation_stock" r:id="rId2"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="disagg building stock" numFmtId="9">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="4.2064379846092042E-5" maxValue="0.1947591919922306"/>
+    </cacheField>
+    <cacheField name="climate reg" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Karachi/Islamabad/Kabul"/>
+        <s v="Java"/>
+        <s v="Busan/Seoul"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Andrea A. Nistad" refreshedDate="43965.626824421299" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="12" xr:uid="{0F12718F-30F6-4BCF-89E7-1B35B81718CD}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="E22:F34" sheet="aggregation_stock" r:id="rId2"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="disagg building stock" numFmtId="9">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.0141665058581035E-2" maxValue="0.50260135135767547"/>
+    </cacheField>
+    <cacheField name="climate reg" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Moscow"/>
+        <s v="Samarkand"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Andrea A. Nistad" refreshedDate="43965.626123263886" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="9" xr:uid="{FF258E16-2918-4CBC-B3E3-6AC27A884314}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="E2:F11" sheet="aggregation_stock" r:id="rId2"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="disagg building stock" numFmtId="9">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.612643328927227E-3" maxValue="0.38348196597904244"/>
+    </cacheField>
+    <cacheField name="climate reg" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Australia"/>
+        <s v="Istanbul"/>
+        <s v="Zurich"/>
+        <s v="Mexico city"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Andrea A. Nistad" refreshedDate="43965.632962152777" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="69" xr:uid="{297EE59C-41D0-444D-A431-21726AA596B4}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="E74:F143" sheet="aggregation_stock" r:id="rId2"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="disagg building stock" numFmtId="9">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="5.893682169665855E-5" maxValue="0.11239790936065834"/>
+    </cacheField>
+    <cacheField name="climate reg" numFmtId="0">
+      <sharedItems count="5">
+        <s v="Cairo"/>
+        <s v="Nigeria"/>
+        <s v="Johannesburg"/>
+        <s v="Teheran "/>
+        <s v="Tel Aviv"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="36">
+  <r>
+    <n v="1.9487440799356817E-4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="8.9710446528055418E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7.7932269048308991E-4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="5.9423251017495619E-4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7.5167776960261825E-4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1.3265355096290864E-4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2.2637703867103523E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="0.42584040981210575"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="9.8968289844978588E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1.0096217091227622E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2.3585397329665997E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1.4823167422537128E-4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2.1412994718526784E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1.3172929757752787E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3.3763753616277516E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="5.435848658407544E-4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2.2826324116787309E-4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="8.3359620548573371E-4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3.3847898390899613E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1.5982842071766681E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2.2274925197673729E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1.8978869223394208E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6.0209529714890025E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7.882426238966097E-4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1.2960736142132128E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="8.2649233136163486E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1.3930228564078049E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6.34594823583325E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1.0663933469667594E-4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3.7306481258398289E-4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2.2728856714556927E-4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1.1644772096898797E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2.8539038511359535E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7.1059838351771225E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6.2649519915250834E-2"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="31">
+  <r>
+    <n v="3.2319600968477274E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="0.11777987688972466"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="5.4865124044498276E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3.1274594307890611E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2.4648356991649124E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="6.5474082346827622E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2.0586641865005223E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.2199695270167802E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="0.1947591919922306"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.8982587449882949E-2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="5.081222715179046E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2.2817069312757725E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3.4289637840563948E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3.9416116359168422E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="4.7615730761712081E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3.9708669048187248E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2.0362875132901685E-2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="2.0431593251337495E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="0.18729220370558908"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6.1113213832474896E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="7.6968940337710026E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="4.2064379846092042E-5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.1458629330246724E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="4.5461806274796677E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.5759650635544721E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.7756701653694182E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="5.1794316527927264E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="9.0171962196897897E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="7.5964021805704696E-5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2.0436568073166402E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="0.14717310622892399"/>
+    <x v="2"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="12">
+  <r>
+    <n v="1.0141665058581035E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3.3357938147025964E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3.2722456307984635E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1.3950115412282107E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6.0914662745149388E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2.0657747778760151E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.4111397740497151E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="0.50260135135767547"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2.9306477530236165E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.9292462104580708E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="0.15572414919524638"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="0.10721957662198076"/>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="9">
+  <r>
+    <n v="0.12953020068336535"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="8.7749592197477674E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.612643328927227E-3"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="3.8961316718818799E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="0.26778117835811976"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="2.4975269334339377E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2.5392267744455271E-2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="4.051556565545409E-2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="0.38348196597904244"/>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="69">
+  <r>
+    <n v="4.0733497680968178E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1.7302584013453973E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="8.5125083600958221E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="6.5625081507315816E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.3159290885677232E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1.1237849106754525E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="6.3044199607288675E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.4456914879120129E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3.2560730901027158E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2.7880651717669537E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="8.7560225918206745E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="4.8240751282616247E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3.0132625186446945E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.4412096560114157E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="5.6714645199674172E-4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="9.4782180317928941E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7.2511445883042679E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2.0742576771183791E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6.2569578275263396E-2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="1.2085644313111557E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.2943005327822638E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.7280756273413085E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.0779572673396481E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="7.0937493137688944E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="8.0478769708182588E-2"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="3.6472568650999376E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="9.5011009812727247E-3"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="2.9709069485214654E-2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="3.9326630147475108E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6.6980168244982988E-3"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="1.2776404141718726E-3"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="2.7750704157634221E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="6.5807563318842294E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1.5037530158058549E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.0390657658280761E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.0820962044752969E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2.5107789703043373E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7.815078030722828E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.4892963342391335E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2.1509174298637274E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1.6779877988838423E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.436423152866537E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1.241126589389091E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="0.11239790936065834"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="4.3753432647134303E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="4.6437886498429531E-3"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="2.6306435827418914E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="5.3572436006364883E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="7.0546384613716755E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.2375423276613095E-4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3.2520419638121911E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="9.0460987804261046E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="5.893682169665855E-5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="4.4502534397159507E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="8.5613264975144942E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3.4367889937759515E-2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="6.6491905325438885E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3.9887543908325301E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="6.8506849530259228E-4"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="1.8452908028941065E-2"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="4.544107695746996E-3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1.1462904723966556E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2.3719337068614475E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="9.4973309199665491E-3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3.1945579181937626E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3.2652008171971651E-4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2.7168516685806918E-2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="9.8533348600801096E-3"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="8.5721469805242149E-3"/>
+    <x v="2"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C1203C04-5A61-4CA0-95DF-55788DF810ED}" name="PivotTable17" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A24:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A2D58C25-0250-44B1-9449-4E6C15D85E4F}" name="PivotTable14" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A4:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C8DA0F9-12D8-49BB-AE44-8AD8E0F4D991}" name="PivotTable13" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A12:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A8FE9055-D368-4FF8-B88E-03C2A8B277BB}" name="PivotTable12" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A18:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="2">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8AA6FF2A-923F-4646-86BA-7D171AD1949F}" name="PivotTable10" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A35:B37" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item n="Rio de Janeiro" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="3">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -630,20 +1814,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFDBA6D-8E3C-C348-8FCA-B609DCB4E55F}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23:B30"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
@@ -1158,6 +2342,188 @@
       </c>
       <c r="C47" s="7">
         <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" t="str">
+        <f>New_regions_climate_reg!A5</f>
+        <v>Australia</v>
+      </c>
+      <c r="C48" s="8">
+        <f>New_regions_climate_reg!B5</f>
+        <v>0.15450547001770473</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" t="str">
+        <f>New_regions_climate_reg!A6</f>
+        <v>Istanbul</v>
+      </c>
+      <c r="C49" s="8">
+        <f>New_regions_climate_reg!B6</f>
+        <v>0.51019287489533893</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" t="str">
+        <f>New_regions_climate_reg!A7</f>
+        <v>Mexico city</v>
+      </c>
+      <c r="C50" s="8">
+        <f>New_regions_climate_reg!B7</f>
+        <v>0.26778117835811976</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" t="str">
+        <f>New_regions_climate_reg!A8</f>
+        <v>Zurich</v>
+      </c>
+      <c r="C51" s="8">
+        <f>New_regions_climate_reg!B8</f>
+        <v>6.7520476728836584E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>94</v>
+      </c>
+      <c r="B52" t="str">
+        <f>New_regions_climate_reg!A13</f>
+        <v>Moscow</v>
+      </c>
+      <c r="C52" s="8">
+        <f>New_regions_climate_reg!B13</f>
+        <v>0.76260907321929272</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" t="str">
+        <f>New_regions_climate_reg!A14</f>
+        <v>Samarkand</v>
+      </c>
+      <c r="C53" s="8">
+        <f>New_regions_climate_reg!B14</f>
+        <v>0.23739092678070717</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54" t="str">
+        <f>New_regions_climate_reg!A19</f>
+        <v>Busan/Seoul</v>
+      </c>
+      <c r="C54" s="8">
+        <f>New_regions_climate_reg!B19</f>
+        <v>0.18651856881170864</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" t="str">
+        <f>New_regions_climate_reg!A20</f>
+        <v>Java</v>
+      </c>
+      <c r="C55" s="8">
+        <f>New_regions_climate_reg!B20</f>
+        <v>0.58910805343805372</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>95</v>
+      </c>
+      <c r="B56" t="str">
+        <f>New_regions_climate_reg!A21</f>
+        <v>Karachi/Islamabad/Kabul</v>
+      </c>
+      <c r="C56" s="8">
+        <f>New_regions_climate_reg!B21</f>
+        <v>0.22437337775023755</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" t="str">
+        <f>New_regions_climate_reg!A25</f>
+        <v>Cairo</v>
+      </c>
+      <c r="C57" s="8">
+        <f>New_regions_climate_reg!B25</f>
+        <v>0.36075719083278696</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" t="str">
+        <f>New_regions_climate_reg!A26</f>
+        <v>Johannesburg</v>
+      </c>
+      <c r="C58" s="8">
+        <f>New_regions_climate_reg!B26</f>
+        <v>0.14703472844831636</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" t="str">
+        <f>New_regions_climate_reg!A27</f>
+        <v>Nigeria</v>
+      </c>
+      <c r="C59" s="8">
+        <f>New_regions_climate_reg!B27</f>
+        <v>0.37243349652615881</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" t="str">
+        <f>New_regions_climate_reg!A28</f>
+        <v xml:space="preserve">Teheran </v>
+      </c>
+      <c r="C60" s="8">
+        <f>GETPIVOTDATA("disagg building stock",New_regions_climate_reg!$A$24,"climate reg","Teheran ")+GETPIVOTDATA("disagg building stock",New_regions_climate_reg!$A$24,"climate reg","Tel Aviv")</f>
+        <v>0.11977458419273762</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" t="str">
+        <f>New_regions_climate_reg!A36</f>
+        <v>Rio de Janeiro</v>
+      </c>
+      <c r="C61" s="8">
+        <f>New_regions_climate_reg!B36</f>
+        <v>0.99999999999999978</v>
       </c>
     </row>
   </sheetData>
@@ -1168,6 +2534,247 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E07E12B2-6BF9-43A3-B2AC-319EDBF96535}">
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75">
+      <c r="A3" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0.15450547001770473</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0.51019287489533893</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0.26778117835811976</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="11">
+        <v>6.7520476728836584E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75">
+      <c r="A11" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="11">
+        <v>0.76260907321929272</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="11">
+        <v>0.23739092678070717</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15">
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75">
+      <c r="A17" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="11">
+        <v>0.18651856881170864</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="11">
+        <v>0.58910805343805372</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="11">
+        <v>0.22437337775023755</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22">
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25">
+        <v>0.36075719083278696</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26">
+        <v>0.14703472844831636</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27">
+        <v>0.37243349652615881</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28">
+        <v>9.8931677737123649E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29">
+        <v>2.0842906455613978E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30">
+        <v>0.99999999999999978</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75">
+      <c r="A34" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="11">
+        <v>0.99999999999999978</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37">
+        <v>0.99999999999999978</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E72D9CB-D67C-E948-8106-77508414AA91}">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -1175,12 +2782,12 @@
       <selection activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="B1" s="6" t="s">
         <v>26</v>
       </c>
@@ -1479,20 +3086,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5019B19B-4BC0-D34F-8472-B5E781AAFF7A}">
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:Q13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="14" width="10.28515625" customWidth="1"/>
+    <col min="2" max="14" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">

</xml_diff>

<commit_message>
adding aggregation of new climate regions
</commit_message>
<xml_diff>
--- a/data/aggregate.xlsx
+++ b/data/aggregate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrenis\gitprojects\BuildME\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF20039B-D27B-429E-8ABA-8C309B67F48E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B4CCE9-927D-4EF0-8B4E-FFA6A623EECF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{464E4639-C8DD-E743-AA72-67524FC7DCD8}"/>
   </bookViews>
@@ -20,11 +20,11 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="17" r:id="rId5"/>
-    <pivotCache cacheId="11" r:id="rId6"/>
-    <pivotCache cacheId="8" r:id="rId7"/>
-    <pivotCache cacheId="5" r:id="rId8"/>
-    <pivotCache cacheId="20" r:id="rId9"/>
+    <pivotCache cacheId="8" r:id="rId5"/>
+    <pivotCache cacheId="9" r:id="rId6"/>
+    <pivotCache cacheId="10" r:id="rId7"/>
+    <pivotCache cacheId="11" r:id="rId8"/>
+    <pivotCache cacheId="12" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="102">
   <si>
     <t>1A-2A</t>
   </si>
@@ -335,6 +335,18 @@
   </si>
   <si>
     <t>Oth-LAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brazil </t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Egypt</t>
   </si>
 </sst>
 </file>
@@ -1237,7 +1249,115 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C1203C04-5A61-4CA0-95DF-55788DF810ED}" name="PivotTable17" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A8FE9055-D368-4FF8-B88E-03C2A8B277BB}" name="PivotTable12" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A18:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8AA6FF2A-923F-4646-86BA-7D171AD1949F}" name="PivotTable10" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A35:B37" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item n="Rio de Janeiro" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C1203C04-5A61-4CA0-95DF-55788DF810ED}" name="PivotTable17" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A24:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" numFmtId="9" showAll="0"/>
@@ -1293,8 +1413,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A2D58C25-0250-44B1-9449-4E6C15D85E4F}" name="PivotTable14" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A2D58C25-0250-44B1-9449-4E6C15D85E4F}" name="PivotTable14" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" numFmtId="9" showAll="0"/>
@@ -1335,118 +1455,6 @@
     <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="0">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C8DA0F9-12D8-49BB-AE44-8AD8E0F4D991}" name="PivotTable13" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A12:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField dataField="1" numFmtId="9" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="1">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A8FE9055-D368-4FF8-B88E-03C2A8B277BB}" name="PivotTable12" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A18:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField dataField="1" numFmtId="9" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
     <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
@@ -1468,13 +1476,14 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8AA6FF2A-923F-4646-86BA-7D171AD1949F}" name="PivotTable10" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A35:B37" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C8DA0F9-12D8-49BB-AE44-8AD8E0F4D991}" name="PivotTable13" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A12:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" numFmtId="9" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="2">
-        <item n="Rio de Janeiro" x="0"/>
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1482,9 +1491,12 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="2">
+  <rowItems count="3">
     <i>
       <x/>
+    </i>
+    <i>
+      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -1818,7 +1830,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
+      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
@@ -2349,182 +2361,68 @@
         <v>93</v>
       </c>
       <c r="B48" t="str">
-        <f>New_regions_climate_reg!A5</f>
-        <v>Australia</v>
+        <f>New_regions_climate_reg!A6</f>
+        <v>Istanbul</v>
       </c>
       <c r="C48" s="8">
-        <f>New_regions_climate_reg!B5</f>
-        <v>0.15450547001770473</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>93</v>
-      </c>
-      <c r="B49" t="str">
-        <f>New_regions_climate_reg!A6</f>
-        <v>Istanbul</v>
+        <v>94</v>
+      </c>
+      <c r="B49" t="s">
+        <v>99</v>
       </c>
       <c r="C49" s="8">
-        <f>New_regions_climate_reg!B6</f>
-        <v>0.51019287489533893</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>93</v>
-      </c>
-      <c r="B50" t="str">
-        <f>New_regions_climate_reg!A7</f>
-        <v>Mexico city</v>
+        <v>95</v>
+      </c>
+      <c r="B50" t="s">
+        <v>100</v>
       </c>
       <c r="C50" s="8">
-        <f>New_regions_climate_reg!B7</f>
-        <v>0.26778117835811976</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>93</v>
-      </c>
-      <c r="B51" t="str">
-        <f>New_regions_climate_reg!A8</f>
-        <v>Zurich</v>
+        <v>96</v>
+      </c>
+      <c r="B51" t="s">
+        <v>101</v>
       </c>
       <c r="C51" s="8">
-        <f>New_regions_climate_reg!B8</f>
-        <v>6.7520476728836584E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>94</v>
-      </c>
-      <c r="B52" t="str">
-        <f>New_regions_climate_reg!A13</f>
-        <v>Moscow</v>
-      </c>
-      <c r="C52" s="8">
-        <f>New_regions_climate_reg!B13</f>
-        <v>0.76260907321929272</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
-        <v>94</v>
-      </c>
-      <c r="B53" t="str">
-        <f>New_regions_climate_reg!A14</f>
-        <v>Samarkand</v>
-      </c>
-      <c r="C53" s="8">
-        <f>New_regions_climate_reg!B14</f>
-        <v>0.23739092678070717</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
-        <v>95</v>
-      </c>
-      <c r="B54" t="str">
-        <f>New_regions_climate_reg!A19</f>
-        <v>Busan/Seoul</v>
-      </c>
-      <c r="C54" s="8">
-        <f>New_regions_climate_reg!B19</f>
-        <v>0.18651856881170864</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>95</v>
-      </c>
-      <c r="B55" t="str">
-        <f>New_regions_climate_reg!A20</f>
-        <v>Java</v>
-      </c>
-      <c r="C55" s="8">
-        <f>New_regions_climate_reg!B20</f>
-        <v>0.58910805343805372</v>
+        <v>97</v>
+      </c>
+      <c r="B52" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" t="s">
-        <v>95</v>
-      </c>
-      <c r="B56" t="str">
-        <f>New_regions_climate_reg!A21</f>
-        <v>Karachi/Islamabad/Kabul</v>
-      </c>
-      <c r="C56" s="8">
-        <f>New_regions_climate_reg!B21</f>
-        <v>0.22437337775023755</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
-        <v>96</v>
-      </c>
-      <c r="B57" t="str">
-        <f>New_regions_climate_reg!A25</f>
-        <v>Cairo</v>
-      </c>
-      <c r="C57" s="8">
-        <f>New_regions_climate_reg!B25</f>
-        <v>0.36075719083278696</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
-        <v>96</v>
-      </c>
-      <c r="B58" t="str">
-        <f>New_regions_climate_reg!A26</f>
-        <v>Johannesburg</v>
-      </c>
-      <c r="C58" s="8">
-        <f>New_regions_climate_reg!B26</f>
-        <v>0.14703472844831636</v>
-      </c>
+      <c r="C56" s="8"/>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" t="s">
-        <v>96</v>
-      </c>
-      <c r="B59" t="str">
-        <f>New_regions_climate_reg!A27</f>
-        <v>Nigeria</v>
-      </c>
-      <c r="C59" s="8">
-        <f>New_regions_climate_reg!B27</f>
-        <v>0.37243349652615881</v>
-      </c>
+      <c r="C59" s="8"/>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" t="s">
-        <v>96</v>
-      </c>
-      <c r="B60" t="str">
-        <f>New_regions_climate_reg!A28</f>
-        <v xml:space="preserve">Teheran </v>
-      </c>
-      <c r="C60" s="8">
-        <f>GETPIVOTDATA("disagg building stock",New_regions_climate_reg!$A$24,"climate reg","Teheran ")+GETPIVOTDATA("disagg building stock",New_regions_climate_reg!$A$24,"climate reg","Tel Aviv")</f>
-        <v>0.11977458419273762</v>
-      </c>
+      <c r="C60" s="8"/>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" t="s">
-        <v>97</v>
-      </c>
-      <c r="B61" t="str">
-        <f>New_regions_climate_reg!A36</f>
-        <v>Rio de Janeiro</v>
-      </c>
-      <c r="C61" s="8">
-        <f>New_regions_climate_reg!B36</f>
-        <v>0.99999999999999978</v>
-      </c>
+      <c r="C61" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
adding additional regions to aggregate.xlsx and in settings.py. updating infiltration values for new regions
</commit_message>
<xml_diff>
--- a/data/aggregate.xlsx
+++ b/data/aggregate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrenis\gitprojects\BuildME\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B4CCE9-927D-4EF0-8B4E-FFA6A623EECF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B464501A-975C-474E-AA40-3D68BE05499E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{464E4639-C8DD-E743-AA72-67524FC7DCD8}"/>
   </bookViews>
@@ -20,11 +20,11 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId5"/>
-    <pivotCache cacheId="9" r:id="rId6"/>
-    <pivotCache cacheId="10" r:id="rId7"/>
-    <pivotCache cacheId="11" r:id="rId8"/>
-    <pivotCache cacheId="12" r:id="rId9"/>
+    <pivotCache cacheId="31" r:id="rId5"/>
+    <pivotCache cacheId="32" r:id="rId6"/>
+    <pivotCache cacheId="33" r:id="rId7"/>
+    <pivotCache cacheId="34" r:id="rId8"/>
+    <pivotCache cacheId="35" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="104">
   <si>
     <t>1A-2A</t>
   </si>
@@ -347,6 +347,12 @@
   </si>
   <si>
     <t>Egypt</t>
+  </si>
+  <si>
+    <t>Oth-MAF-Sub-Sahara</t>
+  </si>
+  <si>
+    <t>Turkey</t>
   </si>
 </sst>
 </file>
@@ -444,7 +450,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0\ %"/>
     </dxf>
@@ -456,6 +462,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0\ %"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0\ %"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1249,7 +1258,123 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A8FE9055-D368-4FF8-B88E-03C2A8B277BB}" name="PivotTable12" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A2D58C25-0250-44B1-9449-4E6C15D85E4F}" name="PivotTable14" cacheId="34" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A4:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C8DA0F9-12D8-49BB-AE44-8AD8E0F4D991}" name="PivotTable13" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A12:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A8FE9055-D368-4FF8-B88E-03C2A8B277BB}" name="PivotTable12" cacheId="32" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A18:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" numFmtId="9" showAll="0"/>
@@ -1286,7 +1411,7 @@
     <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="0">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
@@ -1306,8 +1431,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8AA6FF2A-923F-4646-86BA-7D171AD1949F}" name="PivotTable10" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8AA6FF2A-923F-4646-86BA-7D171AD1949F}" name="PivotTable10" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A35:B37" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" numFmtId="9" showAll="0"/>
@@ -1336,7 +1461,7 @@
     <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="1">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
@@ -1356,8 +1481,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C1203C04-5A61-4CA0-95DF-55788DF810ED}" name="PivotTable17" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C1203C04-5A61-4CA0-95DF-55788DF810ED}" name="PivotTable17" cacheId="35" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A24:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" numFmtId="9" showAll="0"/>
@@ -1401,115 +1526,8 @@
   <dataFields count="1">
     <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A2D58C25-0250-44B1-9449-4E6C15D85E4F}" name="PivotTable14" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A4:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField dataField="1" numFmtId="9" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
-  </dataFields>
   <formats count="1">
-    <format dxfId="2">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C8DA0F9-12D8-49BB-AE44-8AD8E0F4D991}" name="PivotTable13" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A12:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField dataField="1" numFmtId="9" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="3">
+    <format dxfId="4">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
@@ -1830,7 +1848,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
@@ -2360,9 +2378,8 @@
       <c r="A48" t="s">
         <v>93</v>
       </c>
-      <c r="B48" t="str">
-        <f>New_regions_climate_reg!A6</f>
-        <v>Istanbul</v>
+      <c r="B48" t="s">
+        <v>103</v>
       </c>
       <c r="C48" s="8">
         <v>1</v>
@@ -2403,12 +2420,23 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
         <v>97</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>98</v>
       </c>
-      <c r="C52" s="7">
+      <c r="C53" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2436,7 +2464,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2593,7 +2621,7 @@
       <c r="A25" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="7">
         <v>0.36075719083278696</v>
       </c>
     </row>
@@ -2601,7 +2629,7 @@
       <c r="A26" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="7">
         <v>0.14703472844831636</v>
       </c>
     </row>
@@ -2609,7 +2637,7 @@
       <c r="A27" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="7">
         <v>0.37243349652615881</v>
       </c>
     </row>
@@ -2617,7 +2645,7 @@
       <c r="A28" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="7">
         <v>9.8931677737123649E-2</v>
       </c>
     </row>
@@ -2625,7 +2653,7 @@
       <c r="A29" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="7">
         <v>2.0842906455613978E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding values to aggregate.xlsx for the new climate regions
</commit_message>
<xml_diff>
--- a/data/aggregate.xlsx
+++ b/data/aggregate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrenis\gitprojects\BuildME\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B464501A-975C-474E-AA40-3D68BE05499E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734E124C-3B32-47DB-BD68-5CAC4330328D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{464E4639-C8DD-E743-AA72-67524FC7DCD8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{464E4639-C8DD-E743-AA72-67524FC7DCD8}"/>
   </bookViews>
   <sheets>
     <sheet name="climate_reg" sheetId="2" r:id="rId1"/>
@@ -20,11 +20,11 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="31" r:id="rId5"/>
-    <pivotCache cacheId="32" r:id="rId6"/>
-    <pivotCache cacheId="33" r:id="rId7"/>
-    <pivotCache cacheId="34" r:id="rId8"/>
-    <pivotCache cacheId="35" r:id="rId9"/>
+    <pivotCache cacheId="19" r:id="rId5"/>
+    <pivotCache cacheId="20" r:id="rId6"/>
+    <pivotCache cacheId="21" r:id="rId7"/>
+    <pivotCache cacheId="22" r:id="rId8"/>
+    <pivotCache cacheId="23" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="104">
   <si>
     <t>1A-2A</t>
   </si>
@@ -337,9 +337,6 @@
     <t>Oth-LAM</t>
   </si>
   <si>
-    <t xml:space="preserve">Brazil </t>
-  </si>
-  <si>
     <t>Russia</t>
   </si>
   <si>
@@ -353,6 +350,9 @@
   </si>
   <si>
     <t>Turkey</t>
+  </si>
+  <si>
+    <t>Brazil</t>
   </si>
 </sst>
 </file>
@@ -458,13 +458,13 @@
       <numFmt numFmtId="165" formatCode="0.0\ %"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0\ %"/>
+      <numFmt numFmtId="13" formatCode="0\ %"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0\ %"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="13" formatCode="0\ %"/>
+      <numFmt numFmtId="165" formatCode="0.0\ %"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1258,7 +1258,181 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A2D58C25-0250-44B1-9449-4E6C15D85E4F}" name="PivotTable14" cacheId="34" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A8FE9055-D368-4FF8-B88E-03C2A8B277BB}" name="PivotTable12" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A18:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8AA6FF2A-923F-4646-86BA-7D171AD1949F}" name="PivotTable10" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A35:B37" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item n="Rio de Janeiro" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C1203C04-5A61-4CA0-95DF-55788DF810ED}" name="PivotTable17" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A24:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="2">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A2D58C25-0250-44B1-9449-4E6C15D85E4F}" name="PivotTable14" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" numFmtId="9" showAll="0"/>
@@ -1299,168 +1473,6 @@
     <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="0">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C8DA0F9-12D8-49BB-AE44-8AD8E0F4D991}" name="PivotTable13" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A12:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField dataField="1" numFmtId="9" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="1">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A8FE9055-D368-4FF8-B88E-03C2A8B277BB}" name="PivotTable12" cacheId="32" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A18:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField dataField="1" numFmtId="9" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="2">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8AA6FF2A-923F-4646-86BA-7D171AD1949F}" name="PivotTable10" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A35:B37" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField dataField="1" numFmtId="9" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="2">
-        <item n="Rio de Janeiro" x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of disagg building stock" fld="0" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
     <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
@@ -1482,17 +1494,14 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C1203C04-5A61-4CA0-95DF-55788DF810ED}" name="PivotTable17" cacheId="35" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A24:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C8DA0F9-12D8-49BB-AE44-8AD8E0F4D991}" name="PivotTable13" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A12:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" numFmtId="9" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="6">
+      <items count="3">
         <item x="0"/>
-        <item x="2"/>
         <item x="1"/>
-        <item x="3"/>
-        <item x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1500,21 +1509,12 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="3">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
     </i>
     <i t="grand">
       <x/>
@@ -1846,14 +1846,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFDBA6D-8E3C-C348-8FCA-B609DCB4E55F}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48:B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2379,7 +2379,7 @@
         <v>93</v>
       </c>
       <c r="B48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C48" s="8">
         <v>1</v>
@@ -2390,7 +2390,7 @@
         <v>94</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C49" s="8">
         <v>1</v>
@@ -2401,7 +2401,7 @@
         <v>95</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C50" s="8">
         <v>1</v>
@@ -2412,7 +2412,7 @@
         <v>96</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C51" s="8">
         <v>1</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B52" t="s">
         <v>75</v>
@@ -2434,7 +2434,7 @@
         <v>97</v>
       </c>
       <c r="B53" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C53" s="7">
         <v>1</v>
@@ -2702,10 +2702,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E72D9CB-D67C-E948-8106-77508414AA91}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
@@ -3007,6 +3007,126 @@
         <v>0</v>
       </c>
       <c r="F15" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="7">
+        <v>0</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="7">
+        <v>0</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0</v>
+      </c>
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="7">
+        <v>0</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="7">
+        <v>0</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0</v>
+      </c>
+      <c r="F20" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="7">
+        <v>0</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>